<commit_message>
Debugged test cases customer tagging
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Order/customer_tagging_order_test_data.xlsx
+++ b/TestData/Web_POS/Order/customer_tagging_order_test_data.xlsx
@@ -147,7 +147,7 @@
     <t>TC_02</t>
   </si>
   <si>
-    <t xml:space="preserve">307260624YP3 </t>
+    <t>307260624YP3</t>
   </si>
   <si>
     <t xml:space="preserve">usertwop10 </t>
@@ -882,8 +882,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0" topLeftCell="T16">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0" topLeftCell="B19">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>